<commit_message>
Also fixed Datascape processing to handle new transaction types without code changes
</commit_message>
<xml_diff>
--- a/temp/DatascapeLedger.xlsx
+++ b/temp/DatascapeLedger.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>Store</t>
   </si>
@@ -61,112 +61,172 @@
     <t>WZ192</t>
   </si>
   <si>
-    <t>W1239IN76658</t>
-  </si>
-  <si>
-    <t>1919117866</t>
-  </si>
-  <si>
-    <t>7165175553</t>
-  </si>
-  <si>
-    <t>gfeder</t>
+    <t>W1239IN81588</t>
+  </si>
+  <si>
+    <t>1924159604</t>
+  </si>
+  <si>
+    <t>5854802030</t>
+  </si>
+  <si>
+    <t>bsmith</t>
+  </si>
+  <si>
+    <t>Wireless Prepaid Replenishment</t>
+  </si>
+  <si>
+    <t>W1239IN81591</t>
+  </si>
+  <si>
+    <t>1924160433</t>
+  </si>
+  <si>
+    <t>7168304209</t>
+  </si>
+  <si>
+    <t>KBLUEHS</t>
   </si>
   <si>
     <t>Wireless Bill Payment</t>
   </si>
   <si>
-    <t>W1239IN76779</t>
-  </si>
-  <si>
-    <t>1919120431</t>
-  </si>
-  <si>
-    <t>7166985089</t>
-  </si>
-  <si>
-    <t>aszarpa</t>
-  </si>
-  <si>
-    <t>W1239IN76785</t>
-  </si>
-  <si>
-    <t>1919125747</t>
-  </si>
-  <si>
-    <t>7162138397</t>
+    <t>W1239BP29141</t>
+  </si>
+  <si>
+    <t>1924162859</t>
+  </si>
+  <si>
+    <t>7162002143</t>
+  </si>
+  <si>
+    <t>ryanthomas</t>
+  </si>
+  <si>
+    <t>W1239BP29142</t>
+  </si>
+  <si>
+    <t>1924165806</t>
+  </si>
+  <si>
+    <t>2293954998</t>
+  </si>
+  <si>
+    <t>jgala</t>
+  </si>
+  <si>
+    <t>W1239BP29143</t>
+  </si>
+  <si>
+    <t>1924168688</t>
+  </si>
+  <si>
+    <t>7163745338</t>
+  </si>
+  <si>
+    <t>W1239BP29144</t>
+  </si>
+  <si>
+    <t>1924171731</t>
+  </si>
+  <si>
+    <t>7163886225</t>
+  </si>
+  <si>
+    <t>WZ298</t>
+  </si>
+  <si>
+    <t>W1244BP7605</t>
+  </si>
+  <si>
+    <t>1924168932</t>
+  </si>
+  <si>
+    <t>7165372202</t>
+  </si>
+  <si>
+    <t>narnold</t>
   </si>
   <si>
     <t>Device Payment Full Buyout</t>
   </si>
   <si>
-    <t>W1239BP27941</t>
-  </si>
-  <si>
-    <t>1919129133</t>
-  </si>
-  <si>
-    <t>7163432519</t>
-  </si>
-  <si>
-    <t>ryanthomas</t>
-  </si>
-  <si>
-    <t>Wireless Prepaid Replenishment</t>
-  </si>
-  <si>
-    <t>W1239BP27942</t>
-  </si>
-  <si>
-    <t>1919129553</t>
-  </si>
-  <si>
-    <t>7162647246</t>
-  </si>
-  <si>
-    <t>W1239IN76795</t>
-  </si>
-  <si>
-    <t>1919131088</t>
-  </si>
-  <si>
-    <t>7164324278</t>
+    <t>W1244BP7606</t>
+  </si>
+  <si>
+    <t>1924180148</t>
+  </si>
+  <si>
+    <t>7168649341</t>
+  </si>
+  <si>
+    <t>jrospierski</t>
   </si>
   <si>
     <t>WZ299</t>
   </si>
   <si>
-    <t>W1245BP13457</t>
-  </si>
-  <si>
-    <t>1919119163</t>
-  </si>
-  <si>
-    <t>7166974077</t>
-  </si>
-  <si>
-    <t>nhunt</t>
-  </si>
-  <si>
-    <t>W1245BP13458</t>
-  </si>
-  <si>
-    <t>1919127543</t>
-  </si>
-  <si>
-    <t>7165158408</t>
-  </si>
-  <si>
-    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $1,659.99&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $3.60&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $5.25&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $1,661.64&lt;/div&gt;</t>
+    <t>W1245IN43138</t>
+  </si>
+  <si>
+    <t>1924161934</t>
+  </si>
+  <si>
+    <t>7162616254</t>
+  </si>
+  <si>
+    <t>tims</t>
+  </si>
+  <si>
+    <t>W1245IN43140</t>
+  </si>
+  <si>
+    <t>1924162420</t>
+  </si>
+  <si>
+    <t>7169846964</t>
+  </si>
+  <si>
+    <t>W1245BP13918</t>
+  </si>
+  <si>
+    <t>1924173132</t>
+  </si>
+  <si>
+    <t>7164359452</t>
+  </si>
+  <si>
+    <t>mannym</t>
+  </si>
+  <si>
+    <t>W1245BP13919</t>
+  </si>
+  <si>
+    <t>1924177230</t>
+  </si>
+  <si>
+    <t>9282701628</t>
+  </si>
+  <si>
+    <t>W1245BP13920</t>
+  </si>
+  <si>
+    <t>1924179617</t>
+  </si>
+  <si>
+    <t>7165974644</t>
+  </si>
+  <si>
+    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $2,237.55&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $20.40&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $6.75&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: $2,223.90&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div style='text-align: right; font-size: 15px'&gt;Total: null&lt;/div&gt;</t>
@@ -312,7 +372,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -330,16 +390,16 @@
         <v>18</v>
       </c>
       <c r="H2" t="n">
-        <v>1.73</v>
+        <v>35</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="J2" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2.48</v>
+        <v>30.8</v>
       </c>
       <c r="L2"/>
       <c r="M2"/>
@@ -349,7 +409,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -364,10 +424,10 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
-        <v>373.66</v>
+        <v>84.12</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -376,7 +436,7 @@
         <v>0.75</v>
       </c>
       <c r="K3" t="n">
-        <v>374.41</v>
+        <v>84.87</v>
       </c>
       <c r="L3"/>
       <c r="M3"/>
@@ -386,25 +446,25 @@
         <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" t="n">
-        <v>443.24</v>
+        <v>540</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -413,7 +473,7 @@
         <v>0.75</v>
       </c>
       <c r="K4" t="n">
-        <v>443.99</v>
+        <v>540.75</v>
       </c>
       <c r="L4"/>
       <c r="M4"/>
@@ -423,34 +483,34 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H5" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="I5" t="n">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K5" t="n">
-        <v>26.4</v>
+        <v>200.75</v>
       </c>
       <c r="L5"/>
       <c r="M5"/>
@@ -460,7 +520,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -472,13 +532,13 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H6" t="n">
-        <v>325.32</v>
+        <v>135</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -487,7 +547,7 @@
         <v>0.75</v>
       </c>
       <c r="K6" t="n">
-        <v>326.07</v>
+        <v>135.75</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -497,7 +557,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -509,13 +569,13 @@
         <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H7" t="n">
-        <v>100.42</v>
+        <v>449</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -524,7 +584,7 @@
         <v>0.75</v>
       </c>
       <c r="K7" t="n">
-        <v>101.17</v>
+        <v>449.75</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -534,7 +594,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -549,10 +609,10 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="H8" t="n">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -561,7 +621,7 @@
         <v>0.75</v>
       </c>
       <c r="K8" t="n">
-        <v>180.75</v>
+        <v>25.75</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -571,62 +631,247 @@
         <v>38</v>
       </c>
       <c r="B9" s="2">
-        <v>44061</v>
+        <v>44238</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
       </c>
       <c r="H9" t="n">
-        <v>205.62</v>
+        <v>30</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="J9" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>206.37</v>
+        <v>26.4</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="B10" s="2">
+        <v>44238</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="3"/>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="n">
+        <v>296.86</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K10" t="n">
+        <v>297.61</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="n">
+        <v>65</v>
+      </c>
+      <c r="I11" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44238</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="n">
+        <v>121.44</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K12" t="n">
+        <v>122.19</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2">
+        <v>44238</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="n">
+        <v>40</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2">
+        <v>44238</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="n">
+        <v>216.13</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K14" t="n">
+        <v>216.88</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14"/>
+    </row>
+    <row r="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1"/>

</xml_diff>